<commit_message>
Week 10 outcomes and image path updates
</commit_message>
<xml_diff>
--- a/FFL_Data.xlsx
+++ b/FFL_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelrade\Desktop\FFL-Dash-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB463AB-34C6-425F-ACE6-4522D55EFE32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9514365-E70E-4795-8071-E474BBA34BBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A355A56-67D3-4EBE-9422-BA10374FFA74}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="39">
   <si>
     <t>Points Against</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Cooking with Gas</t>
   </si>
   <si>
-    <t>London Bridge is Down</t>
-  </si>
-  <si>
     <t>Dillon Panthers</t>
   </si>
   <si>
@@ -108,15 +105,9 @@
     <t>Team Icons/juju-modified.png</t>
   </si>
   <si>
-    <t>Team Icons/blood-modified.png</t>
-  </si>
-  <si>
     <t>Team Icons/cooking-modified.png</t>
   </si>
   <si>
-    <t>Team Icons/london-modified.png</t>
-  </si>
-  <si>
     <t>Team Icons/dillon-modified.png</t>
   </si>
   <si>
@@ -142,6 +133,18 @@
   </si>
   <si>
     <t>Bye Breece See You in ValHalla</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Dulcich de Leche</t>
+  </si>
+  <si>
+    <t>Team Icons/breece-modified.png</t>
+  </si>
+  <si>
+    <t>Team Icons/dulcich-modified.png</t>
   </si>
 </sst>
 </file>
@@ -501,21 +504,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657FD601-2028-0A4F-BA12-553C96356FC4}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
-    <col min="5" max="5" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -523,21 +526,21 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>116.92</v>
@@ -546,12 +549,12 @@
         <v>111.36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>115.16</v>
@@ -560,12 +563,12 @@
         <v>87.58</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>99.82</v>
@@ -574,12 +577,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>134.52000000000001</v>
@@ -588,12 +591,12 @@
         <v>116.58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>105.42</v>
@@ -602,12 +605,12 @@
         <v>113.88</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>81</v>
@@ -616,12 +619,12 @@
         <v>99.82</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>119.7</v>
@@ -630,12 +633,12 @@
         <v>66.06</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>87.58</v>
@@ -644,12 +647,12 @@
         <v>115.16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>113.88</v>
@@ -658,12 +661,12 @@
         <v>105.42</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>116.58</v>
@@ -672,12 +675,12 @@
         <v>134.52000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>111.36</v>
@@ -686,12 +689,12 @@
         <v>116.92</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
       </c>
       <c r="C13">
         <v>66.06</v>
@@ -700,7 +703,7 @@
         <v>119.7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -714,7 +717,7 @@
         <v>135.18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -728,7 +731,7 @@
         <v>84.6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -742,9 +745,9 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -756,7 +759,7 @@
         <v>129.78</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -770,9 +773,9 @@
         <v>109.42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -784,9 +787,9 @@
         <v>102.88</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -798,9 +801,9 @@
         <v>109.9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -812,9 +815,9 @@
         <v>83.6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -826,9 +829,9 @@
         <v>109.82</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -840,9 +843,9 @@
         <v>140.46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -854,9 +857,9 @@
         <v>115.46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -868,12 +871,12 @@
         <v>125.16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26">
         <v>96.1</v>
@@ -882,12 +885,12 @@
         <v>107.06</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1">
         <v>111.72</v>
@@ -896,12 +899,12 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1">
         <v>115.42</v>
@@ -910,12 +913,12 @@
         <v>100.6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" s="1">
         <v>100.6</v>
@@ -924,12 +927,12 @@
         <v>115.42</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>107.06</v>
@@ -938,12 +941,12 @@
         <v>96.1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>73.86</v>
@@ -952,12 +955,12 @@
         <v>94.88</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="1">
         <v>109.78</v>
@@ -966,12 +969,12 @@
         <v>102.8</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>90.04</v>
@@ -980,12 +983,12 @@
         <v>78.040000000000006</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34">
         <v>94.88</v>
@@ -994,12 +997,12 @@
         <v>73.86</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35">
         <v>73.599999999999994</v>
@@ -1008,12 +1011,12 @@
         <v>111.72</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36">
         <v>102.8</v>
@@ -1022,12 +1025,12 @@
         <v>109.78</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C37">
         <v>78.040000000000006</v>
@@ -1036,12 +1039,12 @@
         <v>90.04</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C38">
         <v>113.28</v>
@@ -1050,12 +1053,12 @@
         <v>83.36</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="1">
         <v>173</v>
@@ -1064,12 +1067,12 @@
         <v>112.18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="1">
         <v>83.36</v>
@@ -1078,12 +1081,12 @@
         <v>113.28</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C41" s="1">
         <v>129.16</v>
@@ -1092,12 +1095,12 @@
         <v>107.98</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1">
         <v>112.18</v>
@@ -1106,12 +1109,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C43" s="1">
         <v>107.98</v>
@@ -1120,12 +1123,12 @@
         <v>129.16</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" s="1">
         <v>159.26</v>
@@ -1134,12 +1137,12 @@
         <v>112.12</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1">
         <v>110</v>
@@ -1148,12 +1151,12 @@
         <v>82.02</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="1">
         <v>116.32</v>
@@ -1162,12 +1165,12 @@
         <v>93.46</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
         <v>17</v>
-      </c>
-      <c r="B47" t="s">
-        <v>18</v>
       </c>
       <c r="C47" s="1">
         <v>112.12</v>
@@ -1176,12 +1179,12 @@
         <v>159.26</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" s="1">
         <v>82.02</v>
@@ -1190,12 +1193,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C49" s="1">
         <v>93.46</v>
@@ -1204,12 +1207,12 @@
         <v>116.32</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C50" s="1">
         <v>116.48</v>
@@ -1218,12 +1221,12 @@
         <v>92.26</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C51" s="1">
         <v>106.52</v>
@@ -1232,12 +1235,12 @@
         <v>73.16</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52" s="1">
         <v>73.16</v>
@@ -1246,12 +1249,12 @@
         <v>106.52</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C53" s="1">
         <v>121.58</v>
@@ -1260,12 +1263,12 @@
         <v>71.959999999999994</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C54" s="1">
         <v>88.7</v>
@@ -1274,12 +1277,12 @@
         <v>162.97999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C55" s="1">
         <v>92.26</v>
@@ -1288,12 +1291,12 @@
         <v>116.48</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C56" s="1">
         <v>162.97999999999999</v>
@@ -1302,12 +1305,12 @@
         <v>88.7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C57" s="1">
         <v>105.04</v>
@@ -1316,12 +1319,12 @@
         <v>99.86</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
         <v>19</v>
-      </c>
-      <c r="B58" t="s">
-        <v>20</v>
       </c>
       <c r="C58" s="1">
         <v>71.959999999999994</v>
@@ -1330,12 +1333,12 @@
         <v>121.58</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C59" s="1">
         <v>99.86</v>
@@ -1344,12 +1347,12 @@
         <v>105.04</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C60" s="1">
         <v>108.34</v>
@@ -1358,12 +1361,12 @@
         <v>139.46</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C61" s="1">
         <v>139.46</v>
@@ -1372,12 +1375,12 @@
         <v>108.34</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C62" s="1">
         <v>126.8</v>
@@ -1386,12 +1389,12 @@
         <v>135.62</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C63" s="1">
         <v>81.819999999999993</v>
@@ -1400,12 +1403,12 @@
         <v>80.28</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C64" s="1">
         <v>111.5</v>
@@ -1414,12 +1417,12 @@
         <v>101.52</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C65" s="1">
         <v>105.4</v>
@@ -1428,12 +1431,12 @@
         <v>62.98</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C66" s="1">
         <v>73.680000000000007</v>
@@ -1442,12 +1445,12 @@
         <v>112.62</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C67" s="1">
         <v>80.28</v>
@@ -1456,12 +1459,12 @@
         <v>81.819999999999993</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C68" s="1">
         <v>101.52</v>
@@ -1470,12 +1473,12 @@
         <v>111.5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C69" s="1">
         <v>112.62</v>
@@ -1484,12 +1487,12 @@
         <v>73.680000000000007</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C70" s="1">
         <v>135.62</v>
@@ -1498,12 +1501,12 @@
         <v>126.8</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C71" s="1">
         <v>86.36</v>
@@ -1512,12 +1515,12 @@
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C72" s="1">
         <v>79.400000000000006</v>
@@ -1526,12 +1529,12 @@
         <v>86.36</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C73" s="1">
         <v>62.98</v>
@@ -1540,12 +1543,12 @@
         <v>105.4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C74" s="1">
         <v>117.34</v>
@@ -1555,12 +1558,12 @@
       </c>
       <c r="E74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C75" s="1">
         <v>133.62</v>
@@ -1570,12 +1573,12 @@
       </c>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C76" s="1">
         <v>108.7</v>
@@ -1585,12 +1588,12 @@
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B77" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C77" s="1">
         <v>106.66</v>
@@ -1600,12 +1603,12 @@
       </c>
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C78" s="1">
         <v>67.260000000000005</v>
@@ -1615,12 +1618,12 @@
       </c>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C79" s="1">
         <v>61.8</v>
@@ -1630,12 +1633,12 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C80" s="1">
         <v>138.72</v>
@@ -1645,12 +1648,12 @@
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C81" s="1">
         <v>93.2</v>
@@ -1660,12 +1663,12 @@
       </c>
       <c r="E81" s="2"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C82" s="1">
         <v>117.42</v>
@@ -1675,12 +1678,12 @@
       </c>
       <c r="E82" s="2"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C83" s="1">
         <v>106.3</v>
@@ -1690,12 +1693,12 @@
       </c>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C84" s="1">
         <v>99.12</v>
@@ -1705,12 +1708,12 @@
       </c>
       <c r="E84" s="2"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C85" s="1">
         <v>90.2</v>
@@ -1720,12 +1723,12 @@
       </c>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>4</v>
       </c>
       <c r="B86" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C86" s="1">
         <v>125.88</v>
@@ -1734,12 +1737,12 @@
         <v>144.68</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C87" s="1">
         <v>47.14</v>
@@ -1748,12 +1751,12 @@
         <v>127.1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C88" s="1">
         <v>90.72</v>
@@ -1762,12 +1765,12 @@
         <v>101.44</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C89" s="1">
         <v>127.1</v>
@@ -1776,12 +1779,12 @@
         <v>47.14</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>7</v>
       </c>
       <c r="B90" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C90" s="1">
         <v>130.24</v>
@@ -1790,12 +1793,12 @@
         <v>92.12</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B91" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C91" s="1">
         <v>113.64</v>
@@ -1804,12 +1807,12 @@
         <v>141.30000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C92" s="1">
         <v>144.28</v>
@@ -1818,12 +1821,12 @@
         <v>109.14</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C93" s="1">
         <v>141.30000000000001</v>
@@ -1832,12 +1835,12 @@
         <v>113.64</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B94" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C94" s="1">
         <v>109.14</v>
@@ -1846,12 +1849,12 @@
         <v>144.28</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C95" s="1">
         <v>92.12</v>
@@ -1860,12 +1863,12 @@
         <v>130.24</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B96" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C96" s="1">
         <v>101.44</v>
@@ -1874,12 +1877,12 @@
         <v>90.72</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C97" s="1">
         <v>144.68</v>
@@ -1888,12 +1891,12 @@
         <v>125.88</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C98" s="1">
         <v>119.44</v>
@@ -1901,16 +1904,14 @@
       <c r="D98" s="1">
         <v>60.2</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C99" s="1">
         <v>60.2</v>
@@ -1918,16 +1919,14 @@
       <c r="D99" s="1">
         <v>119.44</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C100" s="1">
         <v>117.92</v>
@@ -1935,16 +1934,14 @@
       <c r="D100" s="1">
         <v>82.4</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B101" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C101" s="1">
         <v>122.92</v>
@@ -1952,16 +1949,14 @@
       <c r="D101" s="1">
         <v>108.44</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>7</v>
       </c>
       <c r="B102" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C102" s="1">
         <v>102.8</v>
@@ -1969,16 +1964,14 @@
       <c r="D102" s="1">
         <v>107.14</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B103" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C103" s="1">
         <v>99</v>
@@ -1986,16 +1979,14 @@
       <c r="D103" s="1">
         <v>138.5</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C104" s="1">
         <v>108.44</v>
@@ -2003,16 +1994,14 @@
       <c r="D104" s="1">
         <v>122.92</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C105" s="1">
         <v>116.52</v>
@@ -2020,16 +2009,14 @@
       <c r="D105" s="1">
         <v>75.959999999999994</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E105" s="2"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B106" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C106" s="1">
         <v>75.959999999999994</v>
@@ -2037,16 +2024,14 @@
       <c r="D106" s="1">
         <v>116.52</v>
       </c>
-      <c r="E106" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B107" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C107" s="1">
         <v>82.4</v>
@@ -2054,16 +2039,14 @@
       <c r="D107" s="1">
         <v>117.92</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E107" s="2"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B108" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C108" s="1">
         <v>138.5</v>
@@ -2071,16 +2054,14 @@
       <c r="D108" s="1">
         <v>99</v>
       </c>
-      <c r="E108" s="2" t="s">
+      <c r="E108" s="2"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>11</v>
+      </c>
+      <c r="B109" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>12</v>
-      </c>
-      <c r="B109" t="s">
-        <v>36</v>
       </c>
       <c r="C109" s="1">
         <v>107.14</v>
@@ -2088,11 +2069,216 @@
       <c r="D109" s="1">
         <v>102.8</v>
       </c>
-      <c r="E109" s="2" t="s">
+      <c r="E109" s="2"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" t="s">
+        <v>35</v>
+      </c>
+      <c r="C110" s="1">
+        <v>76.7</v>
+      </c>
+      <c r="D110" s="1">
+        <v>125.24</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111" t="s">
+        <v>35</v>
+      </c>
+      <c r="C111" s="1">
+        <v>118.82</v>
+      </c>
+      <c r="D111" s="1">
+        <v>79.8</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" t="s">
+        <v>35</v>
+      </c>
+      <c r="C112" s="1">
+        <v>62.54</v>
+      </c>
+      <c r="D112" s="1">
+        <v>120.06</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>34</v>
       </c>
+      <c r="B113" t="s">
+        <v>35</v>
+      </c>
+      <c r="C113" s="1">
+        <v>119.2</v>
+      </c>
+      <c r="D113" s="1">
+        <v>127.48</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="1">
+        <v>120.06</v>
+      </c>
+      <c r="D114" s="1">
+        <v>62.54</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>36</v>
+      </c>
+      <c r="B115" t="s">
+        <v>35</v>
+      </c>
+      <c r="C115" s="1">
+        <v>96.3</v>
+      </c>
+      <c r="D115" s="1">
+        <v>89.1</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" t="s">
+        <v>35</v>
+      </c>
+      <c r="C116" s="1">
+        <v>125.24</v>
+      </c>
+      <c r="D116" s="1">
+        <v>76.7</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>9</v>
+      </c>
+      <c r="B117" t="s">
+        <v>35</v>
+      </c>
+      <c r="C117" s="1">
+        <v>127.48</v>
+      </c>
+      <c r="D117" s="1">
+        <v>118.17</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>18</v>
+      </c>
+      <c r="B118" t="s">
+        <v>35</v>
+      </c>
+      <c r="C118" s="1">
+        <v>87.24</v>
+      </c>
+      <c r="D118" s="1">
+        <v>125.68</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>16</v>
+      </c>
+      <c r="B119" t="s">
+        <v>35</v>
+      </c>
+      <c r="C119" s="1">
+        <v>89.1</v>
+      </c>
+      <c r="D119" s="1">
+        <v>96.3</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>10</v>
+      </c>
+      <c r="B120" t="s">
+        <v>35</v>
+      </c>
+      <c r="C120" s="1">
+        <v>125.68</v>
+      </c>
+      <c r="D120" s="1">
+        <v>87.24</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>11</v>
+      </c>
+      <c r="B121" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" s="1">
+        <v>79.8</v>
+      </c>
+      <c r="D121" s="1">
+        <v>118.82</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A126:A137">
+    <sortCondition ref="A126"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Week 13 results update
</commit_message>
<xml_diff>
--- a/FFL_Data.xlsx
+++ b/FFL_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelrade\Desktop\FFL-Dash-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CFE0A2-5A97-430C-AA21-3B08460A80E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93200D1-B0CA-4E7F-8604-25A135E53B04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{2A355A56-67D3-4EBE-9422-BA10374FFA74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A355A56-67D3-4EBE-9422-BA10374FFA74}"/>
   </bookViews>
   <sheets>
     <sheet name="Min Table" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="42">
   <si>
     <t>Points Against</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Week 12</t>
+  </si>
+  <si>
+    <t>Week 13</t>
   </si>
 </sst>
 </file>
@@ -518,11 +521,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657FD601-2028-0A4F-BA12-553C96356FC4}">
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E131" sqref="E131"/>
+      <selection pane="bottomLeft" activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2458,9 +2461,6 @@
       <c r="D134" s="1">
         <v>97.56</v>
       </c>
-      <c r="E134" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
@@ -2475,9 +2475,6 @@
       <c r="D135" s="1">
         <v>130.94</v>
       </c>
-      <c r="E135" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
@@ -2492,9 +2489,6 @@
       <c r="D136" s="1">
         <v>115.92</v>
       </c>
-      <c r="E136" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
@@ -2509,9 +2503,6 @@
       <c r="D137" s="1">
         <v>115.22</v>
       </c>
-      <c r="E137" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
@@ -2526,9 +2517,6 @@
       <c r="D138" s="1">
         <v>106.02</v>
       </c>
-      <c r="E138" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
@@ -2543,9 +2531,6 @@
       <c r="D139" s="1">
         <v>92.26</v>
       </c>
-      <c r="E139" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
@@ -2560,9 +2545,6 @@
       <c r="D140" s="1">
         <v>87.24</v>
       </c>
-      <c r="E140" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
@@ -2577,9 +2559,6 @@
       <c r="D141" s="1">
         <v>144.56</v>
       </c>
-      <c r="E141" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
@@ -2594,9 +2573,6 @@
       <c r="D142" s="1">
         <v>131.44</v>
       </c>
-      <c r="E142" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
@@ -2611,9 +2587,6 @@
       <c r="D143" s="1">
         <v>114.16</v>
       </c>
-      <c r="E143" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
@@ -2628,9 +2601,6 @@
       <c r="D144" s="1">
         <v>90.8</v>
       </c>
-      <c r="E144" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
@@ -2645,7 +2615,208 @@
       <c r="D145" s="1">
         <v>114.6</v>
       </c>
-      <c r="E145" t="s">
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>4</v>
+      </c>
+      <c r="B146" t="s">
+        <v>41</v>
+      </c>
+      <c r="C146" s="1">
+        <v>119.14</v>
+      </c>
+      <c r="D146" s="1">
+        <v>81.62</v>
+      </c>
+      <c r="E146" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" t="s">
+        <v>41</v>
+      </c>
+      <c r="C147" s="1">
+        <v>102.1</v>
+      </c>
+      <c r="D147" s="1">
+        <v>98.72</v>
+      </c>
+      <c r="E147" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" t="s">
+        <v>41</v>
+      </c>
+      <c r="C148" s="1">
+        <v>89.74</v>
+      </c>
+      <c r="D148" s="1">
+        <v>74.5</v>
+      </c>
+      <c r="E148" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>33</v>
+      </c>
+      <c r="B149" t="s">
+        <v>41</v>
+      </c>
+      <c r="C149" s="1">
+        <v>115.3</v>
+      </c>
+      <c r="D149" s="1">
+        <v>140.96</v>
+      </c>
+      <c r="E149" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>7</v>
+      </c>
+      <c r="B150" t="s">
+        <v>41</v>
+      </c>
+      <c r="C150" s="1">
+        <v>140.96</v>
+      </c>
+      <c r="D150" s="1">
+        <v>115.3</v>
+      </c>
+      <c r="E150" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>35</v>
+      </c>
+      <c r="B151" t="s">
+        <v>41</v>
+      </c>
+      <c r="C151" s="1">
+        <v>106.78</v>
+      </c>
+      <c r="D151" s="1">
+        <v>120.6</v>
+      </c>
+      <c r="E151" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>8</v>
+      </c>
+      <c r="B152" t="s">
+        <v>41</v>
+      </c>
+      <c r="C152" s="1">
+        <v>123.72</v>
+      </c>
+      <c r="D152" s="1">
+        <v>111.86</v>
+      </c>
+      <c r="E152" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>9</v>
+      </c>
+      <c r="B153" t="s">
+        <v>41</v>
+      </c>
+      <c r="C153" s="1">
+        <v>111.86</v>
+      </c>
+      <c r="D153" s="1">
+        <v>123.72</v>
+      </c>
+      <c r="E153" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>17</v>
+      </c>
+      <c r="B154" t="s">
+        <v>41</v>
+      </c>
+      <c r="C154" s="1">
+        <v>74.5</v>
+      </c>
+      <c r="D154" s="1">
+        <v>89.74</v>
+      </c>
+      <c r="E154" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>15</v>
+      </c>
+      <c r="B155" t="s">
+        <v>41</v>
+      </c>
+      <c r="C155" s="1">
+        <v>81.62</v>
+      </c>
+      <c r="D155" s="1">
+        <v>119.14</v>
+      </c>
+      <c r="E155" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>39</v>
+      </c>
+      <c r="B156" t="s">
+        <v>41</v>
+      </c>
+      <c r="C156" s="1">
+        <v>98.72</v>
+      </c>
+      <c r="D156" s="1">
+        <v>102.1</v>
+      </c>
+      <c r="E156" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>10</v>
+      </c>
+      <c r="B157" t="s">
+        <v>41</v>
+      </c>
+      <c r="C157" s="1">
+        <v>120.6</v>
+      </c>
+      <c r="D157" s="1">
+        <v>106.78</v>
+      </c>
+      <c r="E157" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Week 14 results update
</commit_message>
<xml_diff>
--- a/FFL_Data.xlsx
+++ b/FFL_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelrade\Desktop\FFL-Dash-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93200D1-B0CA-4E7F-8604-25A135E53B04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEBA865-CC3E-4B1D-A901-90AB0D546EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A355A56-67D3-4EBE-9422-BA10374FFA74}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="43">
   <si>
     <t>Points Against</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Week 13</t>
+  </si>
+  <si>
+    <t>Week 14</t>
   </si>
 </sst>
 </file>
@@ -521,11 +524,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657FD601-2028-0A4F-BA12-553C96356FC4}">
-  <dimension ref="A1:E157"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C158" sqref="C158"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2629,9 +2632,6 @@
       <c r="D146" s="1">
         <v>81.62</v>
       </c>
-      <c r="E146" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
@@ -2646,9 +2646,6 @@
       <c r="D147" s="1">
         <v>98.72</v>
       </c>
-      <c r="E147" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
@@ -2663,9 +2660,6 @@
       <c r="D148" s="1">
         <v>74.5</v>
       </c>
-      <c r="E148" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
@@ -2680,9 +2674,6 @@
       <c r="D149" s="1">
         <v>140.96</v>
       </c>
-      <c r="E149" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
@@ -2697,9 +2688,6 @@
       <c r="D150" s="1">
         <v>115.3</v>
       </c>
-      <c r="E150" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
@@ -2714,9 +2702,6 @@
       <c r="D151" s="1">
         <v>120.6</v>
       </c>
-      <c r="E151" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
@@ -2731,9 +2716,6 @@
       <c r="D152" s="1">
         <v>111.86</v>
       </c>
-      <c r="E152" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
@@ -2748,9 +2730,6 @@
       <c r="D153" s="1">
         <v>123.72</v>
       </c>
-      <c r="E153" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
@@ -2765,9 +2744,6 @@
       <c r="D154" s="1">
         <v>89.74</v>
       </c>
-      <c r="E154" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
@@ -2782,9 +2758,6 @@
       <c r="D155" s="1">
         <v>119.14</v>
       </c>
-      <c r="E155" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
@@ -2799,9 +2772,6 @@
       <c r="D156" s="1">
         <v>102.1</v>
       </c>
-      <c r="E156" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
@@ -2816,7 +2786,208 @@
       <c r="D157" s="1">
         <v>106.78</v>
       </c>
-      <c r="E157" t="s">
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>4</v>
+      </c>
+      <c r="B158" t="s">
+        <v>42</v>
+      </c>
+      <c r="C158" s="1">
+        <v>91.16</v>
+      </c>
+      <c r="D158" s="1">
+        <v>76.56</v>
+      </c>
+      <c r="E158" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" t="s">
+        <v>42</v>
+      </c>
+      <c r="C159" s="1">
+        <v>100.08</v>
+      </c>
+      <c r="D159" s="1">
+        <v>107.68</v>
+      </c>
+      <c r="E159" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>6</v>
+      </c>
+      <c r="B160" t="s">
+        <v>42</v>
+      </c>
+      <c r="C160" s="1">
+        <v>85.92</v>
+      </c>
+      <c r="D160" s="1">
+        <v>101.18</v>
+      </c>
+      <c r="E160" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>33</v>
+      </c>
+      <c r="B161" t="s">
+        <v>42</v>
+      </c>
+      <c r="C161" s="1">
+        <v>101.18</v>
+      </c>
+      <c r="D161" s="1">
+        <v>85.92</v>
+      </c>
+      <c r="E161" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>7</v>
+      </c>
+      <c r="B162" t="s">
+        <v>42</v>
+      </c>
+      <c r="C162" s="1">
+        <v>76.56</v>
+      </c>
+      <c r="D162" s="1">
+        <v>91.16</v>
+      </c>
+      <c r="E162" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>35</v>
+      </c>
+      <c r="B163" t="s">
+        <v>42</v>
+      </c>
+      <c r="C163" s="1">
+        <v>109.76</v>
+      </c>
+      <c r="D163" s="1">
+        <v>117.02</v>
+      </c>
+      <c r="E163" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>8</v>
+      </c>
+      <c r="B164" t="s">
+        <v>42</v>
+      </c>
+      <c r="C164" s="1">
+        <v>110.88</v>
+      </c>
+      <c r="D164" s="1">
+        <v>105.6</v>
+      </c>
+      <c r="E164" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>9</v>
+      </c>
+      <c r="B165" t="s">
+        <v>42</v>
+      </c>
+      <c r="C165" s="1">
+        <v>89.62</v>
+      </c>
+      <c r="D165" s="1">
+        <v>115.26</v>
+      </c>
+      <c r="E165" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>17</v>
+      </c>
+      <c r="B166" t="s">
+        <v>42</v>
+      </c>
+      <c r="C166" s="1">
+        <v>117.02</v>
+      </c>
+      <c r="D166" s="1">
+        <v>109.76</v>
+      </c>
+      <c r="E166" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>15</v>
+      </c>
+      <c r="B167" t="s">
+        <v>42</v>
+      </c>
+      <c r="C167" s="1">
+        <v>107.68</v>
+      </c>
+      <c r="D167" s="1">
+        <v>100.08</v>
+      </c>
+      <c r="E167" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>39</v>
+      </c>
+      <c r="B168" t="s">
+        <v>42</v>
+      </c>
+      <c r="C168" s="1">
+        <v>105.6</v>
+      </c>
+      <c r="D168" s="1">
+        <v>110.88</v>
+      </c>
+      <c r="E168" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>10</v>
+      </c>
+      <c r="B169" t="s">
+        <v>42</v>
+      </c>
+      <c r="C169" s="1">
+        <v>115.26</v>
+      </c>
+      <c r="D169" s="1">
+        <v>89.62</v>
+      </c>
+      <c r="E169" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>